<commit_message>
Atualizando o cronograma do projeto
</commit_message>
<xml_diff>
--- a/anotaçõesDoProjeto/cronogramaProjeto.xlsx
+++ b/anotaçõesDoProjeto/cronogramaProjeto.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiwat\.01IOS-Projeto\projetoIntegradorIOS\anotaçõesDoProjeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25D0E45D-1D70-42AB-9CA5-DFEEDA502D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09CBDCF-7C1D-4E6A-849D-1700FAFC5A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{400007A5-1165-4AF5-96AD-A3C8BF0960D7}"/>
+    <workbookView xWindow="10275" yWindow="0" windowWidth="10200" windowHeight="10785" xr2:uid="{400007A5-1165-4AF5-96AD-A3C8BF0960D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -286,30 +285,36 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,58 +325,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="3">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -391,91 +360,11 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -802,7 +691,7 @@
   <dimension ref="A2:BT22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,14 +922,14 @@
       </c>
     </row>
     <row r="3" spans="1:72" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1109,18 +998,18 @@
       <c r="BT3" s="7"/>
     </row>
     <row r="4" spans="1:72" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="4"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -1189,36 +1078,36 @@
       <c r="BT4" s="7"/>
     </row>
     <row r="5" spans="1:72" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="17" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
       <c r="W5" s="9"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="7"/>
@@ -1277,37 +1166,37 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="22" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
       <c r="AH6" s="9"/>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="9"/>
@@ -1371,50 +1260,50 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="23" t="s">
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AI7" s="23"/>
-      <c r="AJ7" s="23"/>
-      <c r="AK7" s="23"/>
-      <c r="AL7" s="23"/>
-      <c r="AM7" s="23"/>
-      <c r="AN7" s="23"/>
-      <c r="AO7" s="23"/>
-      <c r="AP7" s="23"/>
-      <c r="AQ7" s="23"/>
-      <c r="AR7" s="23"/>
-      <c r="AS7" s="23"/>
-      <c r="AT7" s="23"/>
-      <c r="AU7" s="23"/>
-      <c r="AV7" s="23"/>
-      <c r="AW7" s="23"/>
-      <c r="AX7" s="23"/>
-      <c r="AY7" s="23"/>
-      <c r="AZ7" s="23"/>
-      <c r="BA7" s="23"/>
-      <c r="BB7" s="23"/>
-      <c r="BC7" s="23"/>
-      <c r="BD7" s="23"/>
-      <c r="BE7" s="23"/>
-      <c r="BF7" s="23"/>
-      <c r="BG7" s="23"/>
-      <c r="BH7" s="23"/>
-      <c r="BI7" s="23"/>
-      <c r="BJ7" s="23"/>
+      <c r="AI7" s="25"/>
+      <c r="AJ7" s="25"/>
+      <c r="AK7" s="25"/>
+      <c r="AL7" s="25"/>
+      <c r="AM7" s="25"/>
+      <c r="AN7" s="25"/>
+      <c r="AO7" s="25"/>
+      <c r="AP7" s="25"/>
+      <c r="AQ7" s="25"/>
+      <c r="AR7" s="25"/>
+      <c r="AS7" s="25"/>
+      <c r="AT7" s="25"/>
+      <c r="AU7" s="25"/>
+      <c r="AV7" s="25"/>
+      <c r="AW7" s="25"/>
+      <c r="AX7" s="25"/>
+      <c r="AY7" s="25"/>
+      <c r="AZ7" s="25"/>
+      <c r="BA7" s="25"/>
+      <c r="BB7" s="25"/>
+      <c r="BC7" s="25"/>
+      <c r="BD7" s="25"/>
+      <c r="BE7" s="25"/>
+      <c r="BF7" s="25"/>
+      <c r="BG7" s="25"/>
+      <c r="BH7" s="25"/>
+      <c r="BI7" s="25"/>
+      <c r="BJ7" s="25"/>
       <c r="BK7" s="9"/>
       <c r="BL7" s="9"/>
       <c r="BM7" s="9"/>
@@ -1460,44 +1349,44 @@
       <c r="AE8" s="7"/>
       <c r="AF8" s="7"/>
       <c r="AG8" s="7"/>
-      <c r="AH8" s="19" t="s">
+      <c r="AH8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AI8" s="25"/>
-      <c r="AJ8" s="25"/>
-      <c r="AK8" s="25"/>
-      <c r="AL8" s="25"/>
-      <c r="AM8" s="25"/>
-      <c r="AN8" s="25"/>
-      <c r="AO8" s="25"/>
-      <c r="AP8" s="25"/>
-      <c r="AQ8" s="25"/>
-      <c r="AR8" s="25"/>
-      <c r="AS8" s="25"/>
-      <c r="AT8" s="25"/>
-      <c r="AU8" s="25"/>
-      <c r="AV8" s="25"/>
-      <c r="AW8" s="25"/>
-      <c r="AX8" s="25"/>
-      <c r="AY8" s="25"/>
-      <c r="AZ8" s="25"/>
-      <c r="BA8" s="25"/>
-      <c r="BB8" s="25"/>
-      <c r="BC8" s="25"/>
-      <c r="BD8" s="25"/>
-      <c r="BE8" s="25"/>
-      <c r="BF8" s="25"/>
-      <c r="BG8" s="25"/>
-      <c r="BH8" s="25"/>
-      <c r="BI8" s="25"/>
-      <c r="BJ8" s="20"/>
-      <c r="BK8" s="24" t="s">
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
+      <c r="AS8" s="14"/>
+      <c r="AT8" s="14"/>
+      <c r="AU8" s="14"/>
+      <c r="AV8" s="14"/>
+      <c r="AW8" s="14"/>
+      <c r="AX8" s="14"/>
+      <c r="AY8" s="14"/>
+      <c r="AZ8" s="14"/>
+      <c r="BA8" s="14"/>
+      <c r="BB8" s="14"/>
+      <c r="BC8" s="14"/>
+      <c r="BD8" s="14"/>
+      <c r="BE8" s="14"/>
+      <c r="BF8" s="14"/>
+      <c r="BG8" s="14"/>
+      <c r="BH8" s="14"/>
+      <c r="BI8" s="14"/>
+      <c r="BJ8" s="15"/>
+      <c r="BK8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="BL8" s="24"/>
-      <c r="BM8" s="24"/>
-      <c r="BN8" s="24"/>
-      <c r="BO8" s="24"/>
+      <c r="BL8" s="26"/>
+      <c r="BM8" s="26"/>
+      <c r="BN8" s="26"/>
+      <c r="BO8" s="26"/>
       <c r="BP8" s="7"/>
       <c r="BQ8" s="7"/>
       <c r="BR8" s="7"/>
@@ -1567,19 +1456,19 @@
       <c r="BH9" s="7"/>
       <c r="BI9" s="7"/>
       <c r="BJ9" s="7"/>
-      <c r="BK9" s="19" t="s">
+      <c r="BK9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="BL9" s="25"/>
-      <c r="BM9" s="25"/>
-      <c r="BN9" s="25"/>
-      <c r="BO9" s="20"/>
-      <c r="BP9" s="21" t="s">
+      <c r="BL9" s="14"/>
+      <c r="BM9" s="14"/>
+      <c r="BN9" s="14"/>
+      <c r="BO9" s="15"/>
+      <c r="BP9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="BQ9" s="21"/>
-      <c r="BR9" s="21"/>
-      <c r="BS9" s="21"/>
+      <c r="BQ9" s="23"/>
+      <c r="BR9" s="23"/>
+      <c r="BS9" s="23"/>
       <c r="BT9" s="7"/>
     </row>
     <row r="10" spans="1:72" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1650,12 +1539,12 @@
       <c r="BM10" s="7"/>
       <c r="BN10" s="7"/>
       <c r="BO10" s="7"/>
-      <c r="BP10" s="13" t="s">
+      <c r="BP10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="BQ10" s="13"/>
-      <c r="BR10" s="13"/>
-      <c r="BS10" s="13"/>
+      <c r="BQ10" s="16"/>
+      <c r="BR10" s="16"/>
+      <c r="BS10" s="16"/>
       <c r="BT10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1678,6 +1567,8 @@
     <row r="22" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="W7:AG7"/>
+    <mergeCell ref="AH8:BJ8"/>
     <mergeCell ref="BK9:BO9"/>
     <mergeCell ref="BP10:BS10"/>
     <mergeCell ref="C4:D4"/>
@@ -1693,17 +1584,15 @@
     <mergeCell ref="AH7:BJ7"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="G6:V6"/>
-    <mergeCell ref="W7:AG7"/>
-    <mergeCell ref="AH8:BJ8"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fora do prazo">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Fora do prazo">
       <formula>NOT(ISERROR(SEARCH("Fora do prazo",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Pendente">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>